<commit_message>
updated new leagues predictions
</commit_message>
<xml_diff>
--- a/NL/DNK.xlsx
+++ b/NL/DNK.xlsx
@@ -294,6 +294,9 @@
     <t>12</t>
   </si>
   <si>
+    <t>14</t>
+  </si>
+  <si>
     <t>suml6_dnk_gc</t>
   </si>
   <si>
@@ -438,9 +441,6 @@
     <t>17</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
@@ -591,40 +591,40 @@
     <t>Viborg,D D D W W D</t>
   </si>
   <si>
-    <t>Aalborg,3 1 2 1 0 3,(10)</t>
-  </si>
-  <si>
-    <t>Aarhus,1 1 3 2 2 1,(10)</t>
-  </si>
-  <si>
-    <t>Brondby,2 1 2 1 1 1,(8)</t>
-  </si>
-  <si>
-    <t>FC Copenhagen,1 3 2 2 3 1,(12)</t>
-  </si>
-  <si>
-    <t>Midtjylland,1 1 0 2 3 0,(7)</t>
-  </si>
-  <si>
-    <t>Nordsjaelland,1 0 0 0 3 1,(5)</t>
-  </si>
-  <si>
-    <t>Odense,2 2 0 2 2 2,(10)</t>
-  </si>
-  <si>
-    <t>Randers FC,4 0 0 0 0 2,(6)</t>
-  </si>
-  <si>
-    <t>Silkeborg,1 1 3 4 0 1,(10)</t>
-  </si>
-  <si>
-    <t>Sonderjyske,1 1 2 0 2 1,(7)</t>
-  </si>
-  <si>
-    <t>Vejle,1 1 0 3 0 0,(5)</t>
-  </si>
-  <si>
-    <t>Viborg,3 1 1 0 1 2,(8)</t>
+    <t>Aalborg,2 1 2 1 0 1,(7)</t>
+  </si>
+  <si>
+    <t>Aarhus,1 0 1 0 0 2,(4)</t>
+  </si>
+  <si>
+    <t>Brondby,1 1 1 2 3 2,(10)</t>
+  </si>
+  <si>
+    <t>FC Copenhagen,0 0 1 2 2 3,(8)</t>
+  </si>
+  <si>
+    <t>Midtjylland,3 0 2 2 4 3,(14)</t>
+  </si>
+  <si>
+    <t>Nordsjaelland,2 1 1 1 2 2,(9)</t>
+  </si>
+  <si>
+    <t>Odense,2 1 1 1 1 1,(7)</t>
+  </si>
+  <si>
+    <t>Randers FC,1 2 0 2 0 2,(7)</t>
+  </si>
+  <si>
+    <t>Silkeborg,2 4 1 1 1 1,(10)</t>
+  </si>
+  <si>
+    <t>Sonderjyske,0 3 1 1 1 0,(6)</t>
+  </si>
+  <si>
+    <t>Vejle,1 0 2 1 1 2,(7)</t>
+  </si>
+  <si>
+    <t>Viborg,1 2 1 1 2 1,(8)</t>
   </si>
   <si>
     <t>Aalborg,4 2 2 3 3 1,(15)</t>
@@ -4956,10 +4956,10 @@
         <v>362</v>
       </c>
       <c r="BM1" t="s">
+        <v>121</v>
+      </c>
+      <c r="BN1" t="s">
         <v>120</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>119</v>
       </c>
       <c r="BO1" t="s">
         <v>363</v>
@@ -8417,7 +8417,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
         <v>264</v>
@@ -8698,7 +8698,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
         <v>264</v>
@@ -8979,7 +8979,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B16" t="s">
         <v>264</v>
@@ -9260,7 +9260,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
         <v>264</v>
@@ -9541,7 +9541,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B18" t="s">
         <v>264</v>
@@ -10384,7 +10384,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B21" t="s">
         <v>264</v>
@@ -10665,7 +10665,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B22" t="s">
         <v>264</v>
@@ -10946,7 +10946,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s">
         <v>264</v>
@@ -11227,7 +11227,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B24" t="s">
         <v>264</v>
@@ -11508,7 +11508,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B25" t="s">
         <v>264</v>
@@ -11789,7 +11789,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
         <v>264</v>
@@ -12070,7 +12070,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B27" t="s">
         <v>264</v>
@@ -12351,7 +12351,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B28" t="s">
         <v>264</v>
@@ -12632,7 +12632,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B29" t="s">
         <v>264</v>
@@ -12913,7 +12913,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B30" t="s">
         <v>264</v>
@@ -13194,7 +13194,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B31" t="s">
         <v>264</v>
@@ -13475,7 +13475,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B32" t="s">
         <v>264</v>
@@ -42157,7 +42157,7 @@
         <v>143</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E1" t="s">
         <v>1144</v>
@@ -42606,7 +42606,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -42621,7 +42621,7 @@
         <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -42672,19 +42672,19 @@
         <v>17</v>
       </c>
       <c r="Y2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="Z2" t="s">
         <v>18</v>
       </c>
       <c r="AA2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB2" t="s">
         <v>19</v>
       </c>
-      <c r="AB2" t="s">
-        <v>22</v>
-      </c>
       <c r="AC2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -42698,82 +42698,82 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T3" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
+      <c r="AA3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="AB3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S3" t="s">
-        <v>17</v>
-      </c>
-      <c r="T3" t="s">
-        <v>17</v>
-      </c>
-      <c r="U3" t="s">
-        <v>17</v>
-      </c>
-      <c r="V3" t="s">
-        <v>17</v>
-      </c>
-      <c r="W3" t="s">
-        <v>17</v>
-      </c>
-      <c r="X3" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z3" t="s">
+      <c r="AC3" t="s">
         <v>29</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -42784,22 +42784,22 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
       </c>
       <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
         <v>17</v>
@@ -42850,19 +42850,19 @@
         <v>17</v>
       </c>
       <c r="Y4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Z4" t="s">
         <v>29</v>
       </c>
       <c r="AA4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="AC4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
@@ -42873,85 +42873,85 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W5" t="s">
+        <v>17</v>
+      </c>
+      <c r="X5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA5" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" t="s">
-        <v>17</v>
-      </c>
-      <c r="P5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>17</v>
-      </c>
-      <c r="R5" t="s">
-        <v>17</v>
-      </c>
-      <c r="S5" t="s">
-        <v>17</v>
-      </c>
-      <c r="T5" t="s">
-        <v>17</v>
-      </c>
-      <c r="U5" t="s">
-        <v>17</v>
-      </c>
-      <c r="V5" t="s">
-        <v>17</v>
-      </c>
-      <c r="W5" t="s">
-        <v>17</v>
-      </c>
-      <c r="X5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>19</v>
-      </c>
       <c r="AB5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AC5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
@@ -42962,85 +42962,85 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>
       </c>
       <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
         <v>22</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" t="s">
+        <v>17</v>
+      </c>
+      <c r="S6" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" t="s">
+        <v>17</v>
+      </c>
+      <c r="U6" t="s">
+        <v>17</v>
+      </c>
+      <c r="V6" t="s">
+        <v>17</v>
+      </c>
+      <c r="W6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA6" t="s">
         <v>29</v>
       </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>17</v>
-      </c>
-      <c r="R6" t="s">
-        <v>17</v>
-      </c>
-      <c r="S6" t="s">
-        <v>17</v>
-      </c>
-      <c r="T6" t="s">
-        <v>17</v>
-      </c>
-      <c r="U6" t="s">
-        <v>17</v>
-      </c>
-      <c r="V6" t="s">
-        <v>17</v>
-      </c>
-      <c r="W6" t="s">
-        <v>17</v>
-      </c>
-      <c r="X6" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>19</v>
-      </c>
       <c r="AB6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AC6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
@@ -43051,85 +43051,85 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>17</v>
+      </c>
+      <c r="R7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S7" t="s">
+        <v>17</v>
+      </c>
+      <c r="T7" t="s">
+        <v>17</v>
+      </c>
+      <c r="U7" t="s">
+        <v>17</v>
+      </c>
+      <c r="V7" t="s">
+        <v>17</v>
+      </c>
+      <c r="W7" t="s">
+        <v>17</v>
+      </c>
+      <c r="X7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
+      <c r="AA7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC7" t="s">
         <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N7" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" t="s">
-        <v>17</v>
-      </c>
-      <c r="P7" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>17</v>
-      </c>
-      <c r="R7" t="s">
-        <v>17</v>
-      </c>
-      <c r="S7" t="s">
-        <v>17</v>
-      </c>
-      <c r="T7" t="s">
-        <v>17</v>
-      </c>
-      <c r="U7" t="s">
-        <v>17</v>
-      </c>
-      <c r="V7" t="s">
-        <v>17</v>
-      </c>
-      <c r="W7" t="s">
-        <v>17</v>
-      </c>
-      <c r="X7" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8">
@@ -43143,79 +43143,79 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" t="s">
+        <v>17</v>
+      </c>
+      <c r="T8" t="s">
+        <v>17</v>
+      </c>
+      <c r="U8" t="s">
+        <v>17</v>
+      </c>
+      <c r="V8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W8" t="s">
+        <v>17</v>
+      </c>
+      <c r="X8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" t="s">
-        <v>17</v>
-      </c>
-      <c r="N8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O8" t="s">
-        <v>17</v>
-      </c>
-      <c r="P8" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>17</v>
-      </c>
-      <c r="R8" t="s">
-        <v>17</v>
-      </c>
-      <c r="S8" t="s">
-        <v>17</v>
-      </c>
-      <c r="T8" t="s">
-        <v>17</v>
-      </c>
-      <c r="U8" t="s">
-        <v>17</v>
-      </c>
-      <c r="V8" t="s">
-        <v>17</v>
-      </c>
-      <c r="W8" t="s">
-        <v>17</v>
-      </c>
-      <c r="X8" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB8" t="s">
         <v>18</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>21</v>
       </c>
       <c r="AC8" t="s">
         <v>29</v>
@@ -43229,16 +43229,16 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
         <v>29</v>
@@ -43295,19 +43295,19 @@
         <v>17</v>
       </c>
       <c r="Y9" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="Z9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="AA9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC9" t="s">
         <v>29</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -43318,19 +43318,19 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
         <v>18</v>
@@ -43387,16 +43387,16 @@
         <v>86</v>
       </c>
       <c r="Z10" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="AA10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AB10" t="s">
         <v>19</v>
       </c>
       <c r="AC10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -43407,85 +43407,85 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
         <v>18</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>18</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R11" t="s">
+        <v>17</v>
+      </c>
+      <c r="S11" t="s">
+        <v>17</v>
+      </c>
+      <c r="T11" t="s">
+        <v>17</v>
+      </c>
+      <c r="U11" t="s">
+        <v>17</v>
+      </c>
+      <c r="V11" t="s">
+        <v>17</v>
+      </c>
+      <c r="W11" t="s">
+        <v>17</v>
+      </c>
+      <c r="X11" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z11" t="s">
         <v>19</v>
-      </c>
-      <c r="F11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M11" t="s">
-        <v>17</v>
-      </c>
-      <c r="N11" t="s">
-        <v>17</v>
-      </c>
-      <c r="O11" t="s">
-        <v>17</v>
-      </c>
-      <c r="P11" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>17</v>
-      </c>
-      <c r="R11" t="s">
-        <v>17</v>
-      </c>
-      <c r="S11" t="s">
-        <v>17</v>
-      </c>
-      <c r="T11" t="s">
-        <v>17</v>
-      </c>
-      <c r="U11" t="s">
-        <v>17</v>
-      </c>
-      <c r="V11" t="s">
-        <v>17</v>
-      </c>
-      <c r="W11" t="s">
-        <v>17</v>
-      </c>
-      <c r="X11" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>18</v>
       </c>
       <c r="AA11" t="s">
         <v>22</v>
       </c>
       <c r="AB11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AC11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
@@ -43499,82 +43499,82 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
         <v>18</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>17</v>
+      </c>
+      <c r="R12" t="s">
+        <v>17</v>
+      </c>
+      <c r="S12" t="s">
+        <v>17</v>
+      </c>
+      <c r="T12" t="s">
+        <v>17</v>
+      </c>
+      <c r="U12" t="s">
+        <v>17</v>
+      </c>
+      <c r="V12" t="s">
+        <v>17</v>
+      </c>
+      <c r="W12" t="s">
+        <v>17</v>
+      </c>
+      <c r="X12" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC12" t="s">
         <v>29</v>
-      </c>
-      <c r="F12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M12" t="s">
-        <v>17</v>
-      </c>
-      <c r="N12" t="s">
-        <v>17</v>
-      </c>
-      <c r="O12" t="s">
-        <v>17</v>
-      </c>
-      <c r="P12" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>17</v>
-      </c>
-      <c r="R12" t="s">
-        <v>17</v>
-      </c>
-      <c r="S12" t="s">
-        <v>17</v>
-      </c>
-      <c r="T12" t="s">
-        <v>17</v>
-      </c>
-      <c r="U12" t="s">
-        <v>17</v>
-      </c>
-      <c r="V12" t="s">
-        <v>17</v>
-      </c>
-      <c r="W12" t="s">
-        <v>17</v>
-      </c>
-      <c r="X12" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="13">
@@ -43585,22 +43585,22 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" t="s">
         <v>18</v>
-      </c>
-      <c r="H13" t="s">
-        <v>19</v>
       </c>
       <c r="I13" t="s">
         <v>17</v>
@@ -43654,16 +43654,16 @@
         <v>84</v>
       </c>
       <c r="Z13" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="AA13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AB13" t="s">
         <v>19</v>
       </c>
       <c r="AC13" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -43751,19 +43751,19 @@
         <v>77</v>
       </c>
       <c r="Y1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Z1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AA1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AB1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AC1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2">
@@ -43840,7 +43840,7 @@
         <v>17</v>
       </c>
       <c r="Y2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Z2" t="s">
         <v>29</v>
@@ -44927,22 +44927,22 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -45001,22 +45001,22 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
@@ -45075,22 +45075,22 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" t="s">
         <v>97</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>97</v>
-      </c>
-      <c r="G4" t="s">
-        <v>96</v>
-      </c>
-      <c r="H4" t="s">
-        <v>96</v>
       </c>
       <c r="I4" t="s">
         <v>17</v>
@@ -45149,22 +45149,22 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" t="s">
         <v>97</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>97</v>
       </c>
-      <c r="F5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" t="s">
-        <v>96</v>
-      </c>
       <c r="H5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
@@ -45223,22 +45223,22 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
         <v>97</v>
       </c>
-      <c r="E6" t="s">
-        <v>96</v>
-      </c>
       <c r="F6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" t="s">
         <v>97</v>
       </c>
-      <c r="G6" t="s">
-        <v>96</v>
-      </c>
       <c r="H6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I6" t="s">
         <v>17</v>
@@ -45297,22 +45297,22 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" t="s">
         <v>97</v>
       </c>
-      <c r="E7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G7" t="s">
-        <v>96</v>
-      </c>
       <c r="H7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I7" t="s">
         <v>17</v>
@@ -45371,22 +45371,22 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" t="s">
         <v>96</v>
-      </c>
-      <c r="D8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H8" t="s">
-        <v>95</v>
       </c>
       <c r="I8" t="s">
         <v>17</v>
@@ -45445,22 +45445,22 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" t="s">
         <v>96</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" t="s">
         <v>96</v>
       </c>
-      <c r="E9" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" t="s">
-        <v>97</v>
-      </c>
-      <c r="G9" t="s">
-        <v>95</v>
-      </c>
       <c r="H9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I9" t="s">
         <v>17</v>
@@ -45519,22 +45519,22 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" t="s">
         <v>96</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10" t="s">
         <v>96</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>96</v>
-      </c>
-      <c r="F10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G10" t="s">
-        <v>95</v>
-      </c>
-      <c r="H10" t="s">
-        <v>95</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
@@ -45593,22 +45593,22 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" t="s">
         <v>96</v>
-      </c>
-      <c r="E11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" t="s">
-        <v>97</v>
-      </c>
-      <c r="G11" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" t="s">
-        <v>95</v>
       </c>
       <c r="I11" t="s">
         <v>17</v>
@@ -45667,22 +45667,22 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" t="s">
         <v>96</v>
       </c>
-      <c r="D12" t="s">
-        <v>95</v>
-      </c>
       <c r="E12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" t="s">
         <v>97</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>96</v>
       </c>
-      <c r="G12" t="s">
-        <v>95</v>
-      </c>
       <c r="H12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I12" t="s">
         <v>17</v>
@@ -45741,22 +45741,22 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" t="s">
         <v>97</v>
       </c>
-      <c r="D13" t="s">
+      <c r="G13" t="s">
         <v>97</v>
       </c>
-      <c r="E13" t="s">
-        <v>97</v>
-      </c>
-      <c r="F13" t="s">
-        <v>96</v>
-      </c>
-      <c r="G13" t="s">
-        <v>96</v>
-      </c>
       <c r="H13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I13" t="s">
         <v>17</v>
@@ -45892,7 +45892,7 @@
         <v>77</v>
       </c>
       <c r="Y1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2">
@@ -45969,7 +45969,7 @@
         <v>17</v>
       </c>
       <c r="Y2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -46123,7 +46123,7 @@
         <v>17</v>
       </c>
       <c r="Y4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5">
@@ -46277,7 +46277,7 @@
         <v>17</v>
       </c>
       <c r="Y6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7">
@@ -46354,7 +46354,7 @@
         <v>17</v>
       </c>
       <c r="Y7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8">
@@ -46431,7 +46431,7 @@
         <v>17</v>
       </c>
       <c r="Y8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9">
@@ -46508,7 +46508,7 @@
         <v>17</v>
       </c>
       <c r="Y9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10">
@@ -46585,7 +46585,7 @@
         <v>17</v>
       </c>
       <c r="Y10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11">
@@ -46739,7 +46739,7 @@
         <v>17</v>
       </c>
       <c r="Y12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13">
@@ -46816,7 +46816,7 @@
         <v>17</v>
       </c>
       <c r="Y13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -46904,22 +46904,22 @@
         <v>77</v>
       </c>
       <c r="Y1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Z1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AA1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AB1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AC1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AD1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2">
@@ -46930,19 +46930,19 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
@@ -46996,7 +46996,7 @@
         <v>17</v>
       </c>
       <c r="Y2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Z2" t="s">
         <v>22</v>
@@ -47022,19 +47022,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -47088,7 +47088,7 @@
         <v>17</v>
       </c>
       <c r="Y3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z3" t="s">
         <v>29</v>
@@ -47114,10 +47114,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E4" t="s">
         <v>29</v>
@@ -47206,7 +47206,7 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -47497,7 +47497,7 @@
         <v>29</v>
       </c>
       <c r="H8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I8" t="s">
         <v>17</v>
@@ -47580,67 +47580,67 @@
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F9" t="s">
         <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H9" t="s">
+        <v>112</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>17</v>
+      </c>
+      <c r="R9" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9" t="s">
+        <v>17</v>
+      </c>
+      <c r="T9" t="s">
+        <v>17</v>
+      </c>
+      <c r="U9" t="s">
+        <v>17</v>
+      </c>
+      <c r="V9" t="s">
+        <v>17</v>
+      </c>
+      <c r="W9" t="s">
+        <v>17</v>
+      </c>
+      <c r="X9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y9" t="s">
         <v>111</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" t="s">
-        <v>17</v>
-      </c>
-      <c r="O9" t="s">
-        <v>17</v>
-      </c>
-      <c r="P9" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>17</v>
-      </c>
-      <c r="R9" t="s">
-        <v>17</v>
-      </c>
-      <c r="S9" t="s">
-        <v>17</v>
-      </c>
-      <c r="T9" t="s">
-        <v>17</v>
-      </c>
-      <c r="U9" t="s">
-        <v>17</v>
-      </c>
-      <c r="V9" t="s">
-        <v>17</v>
-      </c>
-      <c r="W9" t="s">
-        <v>17</v>
-      </c>
-      <c r="X9" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>110</v>
       </c>
       <c r="Z9" t="s">
         <v>18</v>
@@ -47675,14 +47675,14 @@
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" t="s">
         <v>112</v>
       </c>
-      <c r="H10" t="s">
-        <v>111</v>
-      </c>
       <c r="I10" t="s">
         <v>17</v>
       </c>
@@ -47732,7 +47732,7 @@
         <v>17</v>
       </c>
       <c r="Y10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Z10" t="s">
         <v>18</v>
@@ -47758,7 +47758,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -47773,7 +47773,7 @@
         <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I11" t="s">
         <v>17</v>
@@ -47853,7 +47853,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
@@ -47862,7 +47862,7 @@
         <v>18</v>
       </c>
       <c r="G12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H12" t="s">
         <v>18</v>
@@ -47916,7 +47916,7 @@
         <v>17</v>
       </c>
       <c r="Y12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Z12" t="s">
         <v>18</v>
@@ -48045,40 +48045,40 @@
         <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="N1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2">
@@ -48092,34 +48092,34 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
         <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
         <v>138</v>
       </c>
       <c r="I2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J2" t="s">
         <v>87</v>
       </c>
       <c r="K2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L2" t="s">
         <v>21</v>
       </c>
       <c r="M2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N2" t="s">
         <v>19</v>
@@ -48136,28 +48136,28 @@
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E3" t="s">
         <v>86</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H3" t="s">
         <v>88</v>
       </c>
       <c r="I3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J3" t="s">
         <v>84</v>
       </c>
       <c r="K3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L3" t="s">
         <v>22</v>
@@ -48186,28 +48186,28 @@
         <v>84</v>
       </c>
       <c r="F4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J4" t="s">
         <v>83</v>
       </c>
       <c r="K4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L4" t="s">
         <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N4" t="s">
         <v>18</v>
@@ -48224,34 +48224,34 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E5" t="s">
         <v>85</v>
       </c>
       <c r="F5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H5" t="s">
         <v>88</v>
       </c>
       <c r="I5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J5" t="s">
         <v>83</v>
       </c>
       <c r="K5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L5" t="s">
         <v>19</v>
       </c>
       <c r="M5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N5" t="s">
         <v>19</v>
@@ -48268,16 +48268,16 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E6" t="s">
         <v>83</v>
       </c>
       <c r="F6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G6" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="H6" t="s">
         <v>138</v>
@@ -48286,10 +48286,10 @@
         <v>139</v>
       </c>
       <c r="J6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="L6" t="s">
         <v>21</v>
@@ -48312,34 +48312,34 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G7" t="s">
         <v>138</v>
       </c>
       <c r="H7" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="I7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J7" t="s">
         <v>86</v>
       </c>
       <c r="K7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L7" t="s">
         <v>23</v>
       </c>
       <c r="M7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N7" t="s">
         <v>18</v>
@@ -48356,34 +48356,34 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J8" t="s">
         <v>85</v>
       </c>
       <c r="K8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L8" t="s">
         <v>22</v>
       </c>
       <c r="M8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N8" t="s">
         <v>18</v>
@@ -48400,28 +48400,28 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E9" t="s">
         <v>85</v>
       </c>
       <c r="F9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J9" t="s">
         <v>27</v>
       </c>
       <c r="K9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L9" t="s">
         <v>22</v>
@@ -48444,34 +48444,34 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
         <v>83</v>
       </c>
       <c r="F10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G10" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="H10" t="s">
         <v>138</v>
       </c>
       <c r="I10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J10" t="s">
         <v>85</v>
       </c>
       <c r="K10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L10" t="s">
         <v>84</v>
       </c>
       <c r="M10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N10" t="s">
         <v>22</v>
@@ -48488,34 +48488,34 @@
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E11" t="s">
         <v>83</v>
       </c>
       <c r="F11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G11" t="s">
         <v>139</v>
       </c>
       <c r="H11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J11" t="s">
         <v>85</v>
       </c>
       <c r="K11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L11" t="s">
         <v>22</v>
       </c>
       <c r="M11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N11" t="s">
         <v>18</v>
@@ -48532,34 +48532,34 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E12" t="s">
         <v>84</v>
       </c>
       <c r="F12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G12" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="H12" t="s">
         <v>138</v>
       </c>
       <c r="I12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J12" t="s">
         <v>88</v>
       </c>
       <c r="K12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="L12" t="s">
         <v>27</v>
       </c>
       <c r="M12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N12" t="s">
         <v>19</v>
@@ -48582,22 +48582,22 @@
         <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H13" t="s">
         <v>88</v>
       </c>
       <c r="I13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J13" t="s">
         <v>85</v>
       </c>
       <c r="K13" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L13" t="s">
         <v>23</v>
@@ -48631,13 +48631,13 @@
         <v>141</v>
       </c>
       <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
         <v>96</v>
-      </c>
-      <c r="E1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F1" t="s">
-        <v>95</v>
       </c>
       <c r="G1" t="s">
         <v>142</v>
@@ -48666,7 +48666,7 @@
         <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
         <v>84</v>
@@ -48701,7 +48701,7 @@
         <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
@@ -48716,7 +48716,7 @@
         <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J3" t="s">
         <v>167</v>
@@ -48736,7 +48736,7 @@
         <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E4" t="s">
         <v>86</v>
@@ -48751,7 +48751,7 @@
         <v>154</v>
       </c>
       <c r="I4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J4" t="s">
         <v>168</v>
@@ -48771,7 +48771,7 @@
         <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
         <v>85</v>
@@ -48786,7 +48786,7 @@
         <v>155</v>
       </c>
       <c r="I5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J5" t="s">
         <v>149</v>
@@ -48806,13 +48806,13 @@
         <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E6" t="s">
         <v>83</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G6" t="s">
         <v>149</v>
@@ -48844,7 +48844,7 @@
         <v>86</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F7" t="s">
         <v>84</v>
@@ -48882,7 +48882,7 @@
         <v>83</v>
       </c>
       <c r="F8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G8" t="s">
         <v>151</v>
@@ -48914,7 +48914,7 @@
         <v>84</v>
       </c>
       <c r="E9" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
         <v>86</v>
@@ -48926,7 +48926,7 @@
         <v>150</v>
       </c>
       <c r="I9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J9" t="s">
         <v>153</v>
@@ -48987,10 +48987,10 @@
         <v>88</v>
       </c>
       <c r="F11" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="G11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H11" t="s">
         <v>159</v>
@@ -48999,7 +48999,7 @@
         <v>163</v>
       </c>
       <c r="J11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K11" t="n">
         <v>10.0</v>
@@ -49022,10 +49022,10 @@
         <v>84</v>
       </c>
       <c r="F12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H12" t="s">
         <v>160</v>
@@ -49034,7 +49034,7 @@
         <v>164</v>
       </c>
       <c r="J12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K12" t="n">
         <v>11.0</v>
@@ -49057,10 +49057,10 @@
         <v>87</v>
       </c>
       <c r="F13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H13" t="s">
         <v>147</v>
@@ -49069,7 +49069,7 @@
         <v>165</v>
       </c>
       <c r="J13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K13" t="n">
         <v>12.0</v>

</xml_diff>